<commit_message>
onboard manager can register students from .xlsx
</commit_message>
<xml_diff>
--- a/Kings Educational Centre Data Migration File.xlsx
+++ b/Kings Educational Centre Data Migration File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user1\Documents\KINGS EDUCATIONAL CENTRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\projects\sims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19738286-2D49-4C31-8D69-7F9A1AA6DD0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF5D1C-660E-4B5E-8211-D7D8ABB7C008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,9 +427,6 @@
     <t>OTTO YAI</t>
   </si>
   <si>
-    <t>Graduate</t>
-  </si>
-  <si>
     <t>LINA NYABONI</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>BALANCE BROUGHT FORWARD FROM LAST TERM</t>
+  </si>
+  <si>
+    <t>Play Group</t>
   </si>
 </sst>
 </file>
@@ -718,13 +718,13 @@
   </sheetPr>
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124:C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -733,13 +733,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>2000</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -792,7 +792,7 @@
         <v>5250</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>14000</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -876,7 +876,7 @@
         <v>2700</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -904,7 +904,7 @@
         <v>20250</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -918,7 +918,7 @@
         <v>6250</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -946,7 +946,7 @@
         <v>20000</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -960,7 +960,7 @@
         <v>22600</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -988,7 +988,7 @@
         <v>27400</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -1016,7 +1016,7 @@
         <v>5500</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -1030,7 +1030,7 @@
         <v>4300</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1044,7 +1044,7 @@
         <v>500</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -1058,7 +1058,7 @@
         <v>42495</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -1086,7 +1086,7 @@
         <v>9050</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -1114,7 +1114,7 @@
         <v>2750</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -1128,7 +1128,7 @@
         <v>6500</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1142,7 +1142,7 @@
         <v>6500</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -1156,7 +1156,7 @@
         <v>24850</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -1170,7 +1170,7 @@
         <v>10800</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -1184,7 +1184,7 @@
         <v>1450</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -1198,7 +1198,7 @@
         <v>10750</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -1212,7 +1212,7 @@
         <v>5200</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -1226,7 +1226,7 @@
         <v>600</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -1254,7 +1254,7 @@
         <v>10850</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -1282,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1296,7 +1296,7 @@
         <v>14350</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -1310,7 +1310,7 @@
         <v>6850</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -1324,7 +1324,7 @@
         <v>12900</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -1352,7 +1352,7 @@
         <v>43350</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -1366,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -1394,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -1408,7 +1408,7 @@
         <v>25600</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -1422,7 +1422,7 @@
         <v>4020</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -1436,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -1464,7 +1464,7 @@
         <v>17850</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -1478,7 +1478,7 @@
         <v>22950</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -1492,7 +1492,7 @@
         <v>1850</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -1506,7 +1506,7 @@
         <v>29100</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -1520,7 +1520,7 @@
         <v>25900</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -1534,7 +1534,7 @@
         <v>12850</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -1562,7 +1562,7 @@
         <v>7790</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -1576,7 +1576,7 @@
         <v>6350</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -1590,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -1604,7 +1604,7 @@
         <v>1050</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -1632,7 +1632,7 @@
         <v>9950</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -1688,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -1702,7 +1702,7 @@
         <v>850</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -1716,7 +1716,7 @@
         <v>500</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -1730,7 +1730,7 @@
         <v>3400</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -1744,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -1758,7 +1758,7 @@
         <v>58950</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -1772,7 +1772,7 @@
         <v>2300</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -1800,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
@@ -1814,7 +1814,7 @@
         <v>35350</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -1842,7 +1842,7 @@
         <v>7100</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -1884,7 +1884,7 @@
         <v>25500</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -1898,7 +1898,7 @@
         <v>2000</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -1912,7 +1912,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -1926,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -1940,7 +1940,7 @@
         <v>58850</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -1954,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -1968,7 +1968,7 @@
         <v>12750</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -1982,7 +1982,7 @@
         <v>900</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -1996,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -2010,7 +2010,7 @@
         <v>5550</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D92" t="b">
         <v>1</v>
@@ -2024,7 +2024,7 @@
         <v>30650</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -2066,7 +2066,7 @@
         <v>6650</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -2080,7 +2080,7 @@
         <v>23950</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -2094,7 +2094,7 @@
         <v>11850</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -2108,7 +2108,7 @@
         <v>2550</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -2122,7 +2122,7 @@
         <v>1650</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D101" t="b">
         <v>1</v>
@@ -2150,7 +2150,7 @@
         <v>5000</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -2164,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
@@ -2178,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D104" t="b">
         <v>1</v>
@@ -2192,7 +2192,7 @@
         <v>30200</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -2206,7 +2206,7 @@
         <v>550</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D108" t="b">
         <v>1</v>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -2262,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -2276,7 +2276,7 @@
         <v>19100</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D111" t="b">
         <v>1</v>
@@ -2290,7 +2290,7 @@
         <v>0</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -2304,7 +2304,7 @@
         <v>56700</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D113" t="b">
         <v>1</v>
@@ -2318,7 +2318,7 @@
         <v>52500</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -2332,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -2346,7 +2346,7 @@
         <v>17900</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D116" t="b">
         <v>1</v>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D117" t="b">
         <v>1</v>
@@ -2374,7 +2374,7 @@
         <v>22950</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -2388,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D119" t="b">
         <v>1</v>
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D120" t="b">
         <v>1</v>
@@ -2416,7 +2416,7 @@
         <v>1200</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D121" t="b">
         <v>1</v>
@@ -2430,7 +2430,7 @@
         <v>41425</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D122" t="b">
         <v>1</v>
@@ -2444,7 +2444,7 @@
         <v>4500</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D123" t="b">
         <v>1</v>
@@ -2458,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D124" t="b">
         <v>0</v>
@@ -2466,13 +2466,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B125" s="1">
         <v>22884</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D125" t="b">
         <v>0</v>
@@ -2480,13 +2480,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D126" t="b">
         <v>0</v>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B127" s="1">
         <v>0</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D127" t="b">
         <v>0</v>
@@ -2508,13 +2508,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B128" s="1">
         <v>25984</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D128" t="b">
         <v>0</v>
@@ -2522,13 +2522,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" s="1">
         <v>0</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D129" t="b">
         <v>0</v>
@@ -2536,13 +2536,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" s="1">
         <v>30600</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D130" t="b">
         <v>0</v>
@@ -2550,13 +2550,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B131" s="1">
         <v>0</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D131" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
registered and invoiced students from .xlsx
</commit_message>
<xml_diff>
--- a/Kings Educational Centre Data Migration File.xlsx
+++ b/Kings Educational Centre Data Migration File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\projects\sims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF5D1C-660E-4B5E-8211-D7D8ABB7C008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F39A76-C9ED-4037-8563-0F1E131CE99F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="147">
   <si>
     <t>NAMES</t>
   </si>
@@ -388,9 +388,6 @@
     <t>KENNEDY MURIMI</t>
   </si>
   <si>
-    <t>Grade 8</t>
-  </si>
-  <si>
     <t>JOEL MUTHUVI</t>
   </si>
   <si>
@@ -427,6 +424,9 @@
     <t>OTTO YAI</t>
   </si>
   <si>
+    <t>Graduate</t>
+  </si>
+  <si>
     <t>LINA NYABONI</t>
   </si>
   <si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>Play Group</t>
+  </si>
+  <si>
+    <t>ONBOARDING YEAR</t>
+  </si>
+  <si>
+    <t>ONBOARDING TERM</t>
   </si>
 </sst>
 </file>
@@ -716,19 +722,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124:C131"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,8 +749,14 @@
       <c r="D1" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -755,8 +769,14 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>2022</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -769,8 +789,14 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>2022</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -783,8 +809,14 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>2022</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -797,8 +829,14 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>2022</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -811,8 +849,14 @@
       <c r="D6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>2022</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -825,8 +869,14 @@
       <c r="D7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>2022</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -839,8 +889,14 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>2022</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -853,8 +909,14 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>2022</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -867,8 +929,14 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>2022</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -881,8 +949,14 @@
       <c r="D11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>2022</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -895,8 +969,14 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>2022</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -909,8 +989,14 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>2022</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -923,8 +1009,14 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>2022</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -937,8 +1029,14 @@
       <c r="D15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>2022</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -951,8 +1049,14 @@
       <c r="D16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>2022</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -965,8 +1069,14 @@
       <c r="D17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>2022</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -979,8 +1089,14 @@
       <c r="D18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>2022</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -993,8 +1109,14 @@
       <c r="D19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>2022</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1007,8 +1129,14 @@
       <c r="D20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>2022</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1021,8 +1149,14 @@
       <c r="D21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>2022</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1035,8 +1169,14 @@
       <c r="D22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>2022</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -1049,8 +1189,14 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>2022</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1063,8 +1209,14 @@
       <c r="D24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>2022</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -1077,8 +1229,14 @@
       <c r="D25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>2022</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1091,8 +1249,14 @@
       <c r="D26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>2022</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1105,8 +1269,14 @@
       <c r="D27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>2022</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1119,8 +1289,14 @@
       <c r="D28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>2022</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1133,8 +1309,14 @@
       <c r="D29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>2022</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -1147,8 +1329,14 @@
       <c r="D30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>2022</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1161,8 +1349,14 @@
       <c r="D31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>2022</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1175,8 +1369,14 @@
       <c r="D32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>2022</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -1189,8 +1389,14 @@
       <c r="D33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>2022</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1203,8 +1409,14 @@
       <c r="D34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>2022</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1217,8 +1429,14 @@
       <c r="D35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>2022</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1231,8 +1449,14 @@
       <c r="D36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>2022</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1245,8 +1469,14 @@
       <c r="D37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>2022</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1259,8 +1489,14 @@
       <c r="D38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>2022</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1273,8 +1509,14 @@
       <c r="D39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>2022</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1287,8 +1529,14 @@
       <c r="D40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>2022</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -1301,8 +1549,14 @@
       <c r="D41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>2022</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -1315,8 +1569,14 @@
       <c r="D42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>2022</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -1329,8 +1589,14 @@
       <c r="D43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>2022</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -1343,8 +1609,14 @@
       <c r="D44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>2022</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -1357,8 +1629,14 @@
       <c r="D45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>2022</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -1371,8 +1649,14 @@
       <c r="D46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>2022</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -1385,8 +1669,14 @@
       <c r="D47" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>2022</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1399,8 +1689,14 @@
       <c r="D48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>2022</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -1413,8 +1709,14 @@
       <c r="D49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>2022</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -1427,8 +1729,14 @@
       <c r="D50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>2022</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -1441,8 +1749,14 @@
       <c r="D51" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>2022</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -1455,8 +1769,14 @@
       <c r="D52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>2022</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -1469,8 +1789,14 @@
       <c r="D53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>2022</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -1483,8 +1809,14 @@
       <c r="D54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>2022</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -1497,8 +1829,14 @@
       <c r="D55" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>2022</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -1511,8 +1849,14 @@
       <c r="D56" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>2022</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -1525,8 +1869,14 @@
       <c r="D57" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>2022</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -1539,8 +1889,14 @@
       <c r="D58" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>2022</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -1553,8 +1909,14 @@
       <c r="D59" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>2022</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1567,8 +1929,14 @@
       <c r="D60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>2022</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -1581,8 +1949,14 @@
       <c r="D61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>2022</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -1595,8 +1969,14 @@
       <c r="D62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>2022</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>68</v>
       </c>
@@ -1609,8 +1989,14 @@
       <c r="D63" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>2022</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>69</v>
       </c>
@@ -1623,8 +2009,14 @@
       <c r="D64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>2022</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -1637,8 +2029,14 @@
       <c r="D65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>2022</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -1651,8 +2049,14 @@
       <c r="D66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>2022</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -1665,8 +2069,14 @@
       <c r="D67" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>2022</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -1679,8 +2089,14 @@
       <c r="D68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>2022</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>75</v>
       </c>
@@ -1693,8 +2109,14 @@
       <c r="D69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>2022</v>
+      </c>
+      <c r="F69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -1707,8 +2129,14 @@
       <c r="D70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>2022</v>
+      </c>
+      <c r="F70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>77</v>
       </c>
@@ -1721,8 +2149,14 @@
       <c r="D71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>2022</v>
+      </c>
+      <c r="F71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -1735,8 +2169,14 @@
       <c r="D72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>2022</v>
+      </c>
+      <c r="F72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>
@@ -1749,8 +2189,14 @@
       <c r="D73" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>2022</v>
+      </c>
+      <c r="F73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
@@ -1763,8 +2209,14 @@
       <c r="D74" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>2022</v>
+      </c>
+      <c r="F74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>81</v>
       </c>
@@ -1777,8 +2229,14 @@
       <c r="D75" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>2022</v>
+      </c>
+      <c r="F75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>82</v>
       </c>
@@ -1791,8 +2249,14 @@
       <c r="D76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>2022</v>
+      </c>
+      <c r="F76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>83</v>
       </c>
@@ -1805,8 +2269,14 @@
       <c r="D77" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>2022</v>
+      </c>
+      <c r="F77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>84</v>
       </c>
@@ -1819,8 +2289,14 @@
       <c r="D78" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>2022</v>
+      </c>
+      <c r="F78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
@@ -1833,8 +2309,14 @@
       <c r="D79" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>2022</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>86</v>
       </c>
@@ -1847,8 +2329,14 @@
       <c r="D80" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>2022</v>
+      </c>
+      <c r="F80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -1861,8 +2349,14 @@
       <c r="D81" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <v>2022</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>89</v>
       </c>
@@ -1875,8 +2369,14 @@
       <c r="D82" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>2022</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>90</v>
       </c>
@@ -1889,8 +2389,14 @@
       <c r="D83" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>2022</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>91</v>
       </c>
@@ -1903,8 +2409,14 @@
       <c r="D84" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>2022</v>
+      </c>
+      <c r="F84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>92</v>
       </c>
@@ -1917,8 +2429,14 @@
       <c r="D85" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>2022</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>93</v>
       </c>
@@ -1931,8 +2449,14 @@
       <c r="D86" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>2022</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>94</v>
       </c>
@@ -1945,8 +2469,14 @@
       <c r="D87" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>2022</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>95</v>
       </c>
@@ -1959,8 +2489,14 @@
       <c r="D88" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>2022</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>96</v>
       </c>
@@ -1973,8 +2509,14 @@
       <c r="D89" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>2022</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>97</v>
       </c>
@@ -1987,8 +2529,14 @@
       <c r="D90" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>2022</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>98</v>
       </c>
@@ -2001,8 +2549,14 @@
       <c r="D91" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>2022</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>99</v>
       </c>
@@ -2015,8 +2569,14 @@
       <c r="D92" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>2022</v>
+      </c>
+      <c r="F92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>101</v>
       </c>
@@ -2029,8 +2589,14 @@
       <c r="D93" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>2022</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>102</v>
       </c>
@@ -2043,8 +2609,14 @@
       <c r="D94" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>2022</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>103</v>
       </c>
@@ -2057,8 +2629,14 @@
       <c r="D95" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>2022</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>104</v>
       </c>
@@ -2071,8 +2649,14 @@
       <c r="D96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>2022</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>105</v>
       </c>
@@ -2085,8 +2669,14 @@
       <c r="D97" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>2022</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>106</v>
       </c>
@@ -2099,8 +2689,14 @@
       <c r="D98" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>2022</v>
+      </c>
+      <c r="F98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>107</v>
       </c>
@@ -2113,8 +2709,14 @@
       <c r="D99" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>2022</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>109</v>
       </c>
@@ -2127,8 +2729,14 @@
       <c r="D100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>2022</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>110</v>
       </c>
@@ -2141,8 +2749,14 @@
       <c r="D101" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>2022</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>111</v>
       </c>
@@ -2155,8 +2769,14 @@
       <c r="D102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>2022</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>112</v>
       </c>
@@ -2169,8 +2789,14 @@
       <c r="D103" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>2022</v>
+      </c>
+      <c r="F103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>113</v>
       </c>
@@ -2183,8 +2809,14 @@
       <c r="D104" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>2022</v>
+      </c>
+      <c r="F104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>114</v>
       </c>
@@ -2197,8 +2829,14 @@
       <c r="D105" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>2022</v>
+      </c>
+      <c r="F105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>115</v>
       </c>
@@ -2211,8 +2849,14 @@
       <c r="D106" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>2022</v>
+      </c>
+      <c r="F106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>116</v>
       </c>
@@ -2225,8 +2869,14 @@
       <c r="D107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>2022</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>117</v>
       </c>
@@ -2239,8 +2889,14 @@
       <c r="D108" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>2022</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>118</v>
       </c>
@@ -2253,8 +2909,14 @@
       <c r="D109" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>2022</v>
+      </c>
+      <c r="F109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>119</v>
       </c>
@@ -2267,8 +2929,14 @@
       <c r="D110" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>2022</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>120</v>
       </c>
@@ -2281,8 +2949,14 @@
       <c r="D111" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>2022</v>
+      </c>
+      <c r="F111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>121</v>
       </c>
@@ -2295,10 +2969,16 @@
       <c r="D112" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>2022</v>
+      </c>
+      <c r="F112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B113" s="1">
         <v>56700</v>
@@ -2309,10 +2989,16 @@
       <c r="D113" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>2022</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B114" s="1">
         <v>52500</v>
@@ -2323,10 +3009,16 @@
       <c r="D114" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>2022</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B115" s="1">
         <v>0</v>
@@ -2337,10 +3029,16 @@
       <c r="D115" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>2022</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" s="1">
         <v>17900</v>
@@ -2351,10 +3049,16 @@
       <c r="D116" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <v>2022</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B117" s="1">
         <v>0</v>
@@ -2365,10 +3069,16 @@
       <c r="D117" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <v>2022</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B118" s="1">
         <v>22950</v>
@@ -2379,10 +3089,16 @@
       <c r="D118" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <v>2022</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1">
         <v>0</v>
@@ -2393,10 +3109,16 @@
       <c r="D119" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <v>2022</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B120" s="1">
         <v>0</v>
@@ -2407,10 +3129,16 @@
       <c r="D120" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <v>2022</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B121" s="1">
         <v>1200</v>
@@ -2421,10 +3149,16 @@
       <c r="D121" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <v>2022</v>
+      </c>
+      <c r="F121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B122" s="1">
         <v>41425</v>
@@ -2435,10 +3169,16 @@
       <c r="D122" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E122">
+        <v>2022</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123" s="1">
         <v>4500</v>
@@ -2449,22 +3189,34 @@
       <c r="D123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <v>2022</v>
+      </c>
+      <c r="F123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B124" s="1">
-        <v>0</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="D124" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124">
+        <v>2022</v>
+      </c>
+      <c r="F124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>135</v>
       </c>
@@ -2472,13 +3224,19 @@
         <v>22884</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D125" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125">
+        <v>2022</v>
+      </c>
+      <c r="F125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>136</v>
       </c>
@@ -2486,13 +3244,19 @@
         <v>0</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D126" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E126">
+        <v>2022</v>
+      </c>
+      <c r="F126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>137</v>
       </c>
@@ -2500,13 +3264,19 @@
         <v>0</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D127" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E127">
+        <v>2022</v>
+      </c>
+      <c r="F127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>138</v>
       </c>
@@ -2514,13 +3284,19 @@
         <v>25984</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D128" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128">
+        <v>2022</v>
+      </c>
+      <c r="F128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>139</v>
       </c>
@@ -2528,13 +3304,19 @@
         <v>0</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D129" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129">
+        <v>2022</v>
+      </c>
+      <c r="F129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>140</v>
       </c>
@@ -2542,13 +3324,19 @@
         <v>30600</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D130" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130">
+        <v>2022</v>
+      </c>
+      <c r="F130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>141</v>
       </c>
@@ -2556,10 +3344,16 @@
         <v>0</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D131" t="b">
         <v>0</v>
+      </c>
+      <c r="E131">
+        <v>2022</v>
+      </c>
+      <c r="F131">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>